<commit_message>
Can access sheet by subscript.
</commit_message>
<xml_diff>
--- a/tests/workbook_simple.xlsx
+++ b/tests/workbook_simple.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\nik\dev\consult-llm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\nik\dev\excel-helper\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19403099-EC29-43C1-B0D6-DC4D850A0A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DA58C5-7B43-498A-B4EE-0A12A0B18096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14856" xr2:uid="{7FC82244-8FAC-4835-A469-849F33463F01}"/>
+    <workbookView xWindow="-15" yWindow="-18120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{7FC82244-8FAC-4835-A469-849F33463F01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,9 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Quote</t>
+  </si>
+  <si>
+    <t>This is sheet 2</t>
   </si>
 </sst>
 </file>
@@ -412,7 +416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D821DD9D-9ED5-4218-8A68-F1C9ADD639D8}">
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -426,4 +430,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE9D7A6-6E4B-4942-BCF3-5089C2029057}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>